<commit_message>
[IMP] notify_benefit_template.xml renamed to notify_codes_benefit_template, Plantilla_Beneficiarias_Colabora.xlsx now has a level field rather than quantity of products
</commit_message>
<xml_diff>
--- a/rvc/static/xls/Plantilla_Beneficiarias_Colabora.xlsx
+++ b/rvc/static/xls/Plantilla_Beneficiarias_Colabora.xlsx
@@ -28,7 +28,7 @@
     <t xml:space="preserve">Nit Halonadora</t>
   </si>
   <si>
-    <t xml:space="preserve">Cantidad Productos</t>
+    <t xml:space="preserve">Nivel (1 a 10)</t>
   </si>
   <si>
     <t xml:space="preserve">Nombre Contacto</t>
@@ -148,7 +148,7 @@
   <tableColumns count="7">
     <tableColumn id="1" name="Nit Beneficiaria"/>
     <tableColumn id="2" name="Nit Halonadora"/>
-    <tableColumn id="3" name="Cantidad Productos"/>
+    <tableColumn id="3" name="Nivel (1 a 10)"/>
     <tableColumn id="4" name="Nombre Contacto"/>
     <tableColumn id="5" name="Correo Contacto"/>
     <tableColumn id="6" name="Teléfono Contacto"/>
@@ -168,7 +168,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.85"/>

</xml_diff>